<commit_message>
Account and login can be created:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56B90A7-2C62-4961-8AB5-D99CE8131B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C570B42F-D463-4D19-914A-D1F60D7D7737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13950" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -509,6 +509,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,10 +534,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,7 +754,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -862,22 +862,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.666666666666667</c:v>
+                  <c:v>15.833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3333333333333339</c:v>
+                  <c:v>12.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0000000000000009</c:v>
+                  <c:v>9.5000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6666666666666679</c:v>
+                  <c:v>6.3333333333333357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3333333333333346</c:v>
+                  <c:v>3.1666666666666692</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -970,22 +970,22 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1621,7 +1621,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1837,22 +1837,22 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="B2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!G$3:G$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!H$3:H$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="B3" s="1">
         <f>SUM(B10:B11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:H3" si="0">SUM(C10:C11)</f>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="B4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!G$3:G$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!H$3:H$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="B11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!G3:G1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!H3:H1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
@@ -4981,9 +4981,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5000,44 +5000,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="20" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="M2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="21"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -5085,7 +5085,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -5100,7 +5100,7 @@
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="20" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="7" t="str" cm="1">
@@ -5112,7 +5112,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5139,7 +5139,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -10749,7 +10749,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10779,9 +10779,9 @@
       <c r="A2" s="19">
         <v>45262</v>
       </c>
-      <c r="B2" s="28">
-        <f>COUNT('Sprint 1 backlog'!C3:C10)</f>
-        <v>8</v>
+      <c r="B2" s="21">
+        <f>COUNT('Sprint 1 backlog'!C3:C300)</f>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <f>COUNT('Sprint 1 backlog'!C3:C100)</f>
@@ -10789,20 +10789,20 @@
       </c>
       <c r="D2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!G3:G23,"Done")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>45263</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="21">
         <f t="shared" ref="B3:B8" si="0">B2-($B$2/6)</f>
-        <v>6.666666666666667</v>
+        <v>15.833333333333334</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C8" si="1">C2-D3</f>
-        <v>19</v>
+        <f>C2-D2</f>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <f>COUNTIF('Sprint 1 backlog'!H3:H23,"Done")</f>
@@ -10813,13 +10813,13 @@
       <c r="A4" s="19">
         <v>45264</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="21">
         <f t="shared" si="0"/>
-        <v>5.3333333333333339</v>
+        <v>12.666666666666668</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" ref="C4:C8" si="1">C3-D3</f>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!I3:I23,"Done")</f>
@@ -10830,13 +10830,13 @@
       <c r="A5" s="19">
         <v>45265</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="21">
         <f t="shared" si="0"/>
-        <v>4.0000000000000009</v>
+        <v>9.5000000000000018</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <f>COUNTIF('Sprint 1 backlog'!J3:J23,"Done")</f>
@@ -10847,13 +10847,13 @@
       <c r="A6" s="19">
         <v>45266</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="21">
         <f t="shared" si="0"/>
-        <v>2.6666666666666679</v>
+        <v>6.3333333333333357</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <f>COUNTIF('Sprint 1 backlog'!K3:K23,"Done")</f>
@@ -10864,13 +10864,13 @@
       <c r="A7" s="19">
         <v>45267</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="21">
         <f t="shared" si="0"/>
-        <v>1.3333333333333346</v>
+        <v>3.1666666666666692</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
@@ -10881,13 +10881,13 @@
       <c r="A8" s="19">
         <v>45268</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>
@@ -10939,44 +10939,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="20" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="13" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
@@ -10998,7 +10998,7 @@
       <c r="M2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="21"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -11039,7 +11039,7 @@
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="20" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="7" t="str" cm="1">
@@ -15714,7 +15714,7 @@
         <v/>
       </c>
       <c r="C259" s="6" t="str">
-        <f t="shared" ref="C259:C322" si="4">IF(ISBLANK(A259),"",IF(A259&lt;&gt;A258,A259+0.1,C258+0.1))</f>
+        <f t="shared" ref="C259:C300" si="4">IF(ISBLANK(A259),"",IF(A259&lt;&gt;A258,A259+0.1,C258+0.1))</f>
         <v/>
       </c>
       <c r="E259" s="7" t="str" cm="1">
@@ -16560,7 +16560,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16590,7 +16590,7 @@
       <c r="A2" s="19">
         <v>45262</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="21">
         <f>COUNT('Sprint 1 backlog'!C3:C10)</f>
         <v>8</v>
       </c>
@@ -16600,20 +16600,20 @@
       </c>
       <c r="D2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!G3:G23,"Done")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>45263</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="21">
         <f t="shared" ref="B3:B8" si="0">B2-($B$2/6)</f>
         <v>6.666666666666667</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C8" si="1">C2-D3</f>
-        <v>19</v>
+        <f>C2-D2</f>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <f>COUNTIF('Sprint 1 backlog'!H3:H23,"Done")</f>
@@ -16624,13 +16624,13 @@
       <c r="A4" s="19">
         <v>45264</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="21">
         <f t="shared" si="0"/>
         <v>5.3333333333333339</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" ref="C4:C8" si="1">C3-D3</f>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!I3:I23,"Done")</f>
@@ -16641,13 +16641,13 @@
       <c r="A5" s="19">
         <v>45265</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="21">
         <f t="shared" si="0"/>
         <v>4.0000000000000009</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <f>COUNTIF('Sprint 1 backlog'!J3:J23,"Done")</f>
@@ -16658,13 +16658,13 @@
       <c r="A6" s="19">
         <v>45266</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="21">
         <f t="shared" si="0"/>
         <v>2.6666666666666679</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <f>COUNTIF('Sprint 1 backlog'!K3:K23,"Done")</f>
@@ -16675,13 +16675,13 @@
       <c r="A7" s="19">
         <v>45267</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="21">
         <f t="shared" si="0"/>
         <v>1.3333333333333346</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
@@ -16692,13 +16692,13 @@
       <c r="A8" s="19">
         <v>45268</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>
@@ -17262,14 +17262,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d12b44e9-a355-4801-8c10-af0fa875eb52" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5517439e-c63d-4269-a460-349c4f0e575b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17456,21 +17454,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d12b44e9-a355-4801-8c10-af0fa875eb52" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5517439e-c63d-4269-a460-349c4f0e575b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d12b44e9-a355-4801-8c10-af0fa875eb52"/>
-    <ds:schemaRef ds:uri="5517439e-c63d-4269-a460-349c4f0e575b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17495,9 +17492,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d12b44e9-a355-4801-8c10-af0fa875eb52"/>
+    <ds:schemaRef ds:uri="5517439e-c63d-4269-a460-349c4f0e575b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added assembly reference for API to use AdminPortal.Models:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\WebComA3\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\jake\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE9928C-08E7-42C2-9F2B-49C4FABAAC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EB7C5B-96F5-4DAA-9A3C-7C046432553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13950" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="2205" windowWidth="14835" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -20329,6 +20329,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100368EC63562010C468CBEB7AB90BFA937" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbcd4c9f600c040763b05b627a98747d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5517439e-c63d-4269-a460-349c4f0e575b" xmlns:ns3="d12b44e9-a355-4801-8c10-af0fa875eb52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3ca6a824aa0a87c5592ba6780ee9405" ns2:_="" ns3:_="">
     <xsd:import namespace="5517439e-c63d-4269-a460-349c4f0e575b"/>
@@ -20511,15 +20520,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
   <ds:schemaRefs>
@@ -20532,6 +20532,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{759CF7A7-ED7B-4C51-82F1-9078416C083C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20548,12 +20556,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added api function to get single articl:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\jake\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EB7C5B-96F5-4DAA-9A3C-7C046432553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EA6763-F5D3-4DF7-9D4D-B5D189719C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2205" windowWidth="14835" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
   <si>
     <t>Product backlog ID</t>
   </si>
@@ -7597,7 +7597,7 @@
       </c>
       <c r="F2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!K$3:K$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
@@ -7631,11 +7631,11 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="0"/>
@@ -7731,11 +7731,11 @@
       </c>
       <c r="F10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!K3:K1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="G11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
@@ -7785,9 +7785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7795,7 +7794,7 @@
     <col min="1" max="1" width="9.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="60.875" style="6" customWidth="1"/>
     <col min="3" max="3" width="11" style="6" customWidth="1"/>
-    <col min="4" max="4" width="111.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="61.125" style="6" customWidth="1"/>
     <col min="5" max="5" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="13" width="10.375" style="6" customWidth="1"/>
@@ -8228,8 +8227,12 @@
       <c r="J12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="K12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>11</v>
+      </c>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
     </row>
@@ -8268,8 +8271,12 @@
       <c r="J13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="K13" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
     </row>
@@ -8308,7 +8315,9 @@
       <c r="J14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
@@ -8348,8 +8357,12 @@
       <c r="J15" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="K15" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
     </row>
@@ -8388,7 +8401,9 @@
       <c r="J16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
@@ -8468,7 +8483,9 @@
       <c r="J18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="22"/>
+      <c r="K18" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>

</xml_diff>

<commit_message>
Working on blog smmary cards:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\jake\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EA6763-F5D3-4DF7-9D4D-B5D189719C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0F3818-1402-4D4F-AE58-1E7C57C756DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="76">
   <si>
     <t>Product backlog ID</t>
   </si>
@@ -886,7 +886,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1102,7 +1102,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,7 +1753,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1969,7 +1969,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M$3:M$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="G4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M$3:M$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="G10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="G11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A11)</f>
@@ -7786,7 +7786,7 @@
   <dimension ref="A1:N310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8231,7 +8231,7 @@
         <v>26</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
@@ -8318,7 +8318,9 @@
       <c r="K14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
     </row>
@@ -8361,7 +8363,7 @@
         <v>26</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -8404,7 +8406,9 @@
       <c r="K16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="22"/>
+      <c r="L16" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
     </row>
@@ -8486,7 +8490,9 @@
       <c r="K18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="22"/>
+      <c r="L18" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
     </row>
@@ -13822,7 +13828,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13947,7 +13953,7 @@
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -13960,7 +13966,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>
@@ -19758,7 +19764,7 @@
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -19771,7 +19777,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>

</xml_diff>

<commit_message>
Blog can show a single article selected with the url parameters:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\jake\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0F3818-1402-4D4F-AE58-1E7C57C756DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A24C12-0303-49D9-B08B-115A7C22A036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,13 +293,13 @@
     <t>View an account's profile information on the Admin Portal</t>
   </si>
   <si>
-    <t>Create a view to update the article list on the Admin Portal</t>
-  </si>
-  <si>
     <t>Publish an Article</t>
   </si>
   <si>
     <t>Secure the Admin Portal</t>
+  </si>
+  <si>
+    <t>Create a view to update an article on the Admin Portal</t>
   </si>
 </sst>
 </file>
@@ -4189,7 +4189,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="18" t="str">
         <f t="shared" si="2"/>
@@ -4212,7 +4212,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="18" t="str">
         <f t="shared" si="2"/>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M$3:M$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="0"/>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="G10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
@@ -7785,8 +7785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8275,7 +8275,7 @@
         <v>26</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
@@ -8363,7 +8363,7 @@
         <v>26</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -8465,7 +8465,7 @@
         <v>6.1999999999999993</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E18" s="24" t="str" cm="1">
         <f t="array" ref="E18">IF(ISBLANK(A18),"",_xlfn._xlws.FILTER(_xlfn._xlws.FILTER('Product backlog'!$A$2:$C$279,'Product backlog'!$A$2:$A$279=A18),{0,0,1}))</f>
@@ -20352,15 +20352,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100368EC63562010C468CBEB7AB90BFA937" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbcd4c9f600c040763b05b627a98747d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5517439e-c63d-4269-a460-349c4f0e575b" xmlns:ns3="d12b44e9-a355-4801-8c10-af0fa875eb52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3ca6a824aa0a87c5592ba6780ee9405" ns2:_="" ns3:_="">
     <xsd:import namespace="5517439e-c63d-4269-a460-349c4f0e575b"/>
@@ -20543,6 +20534,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
   <ds:schemaRefs>
@@ -20555,14 +20555,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{759CF7A7-ED7B-4C51-82F1-9078416C083C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20579,4 +20571,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added view to update articles on the admin portal:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\jake\WebComA3\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A24C12-0303-49D9-B08B-115A7C22A036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7448C6-F58D-4EA0-9731-728F34508165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -886,7 +886,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1102,7 +1102,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,7 +1753,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1969,7 +1969,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3842,9 +3842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3979,7 +3979,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>49</v>
@@ -4004,7 +4004,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>50</v>
@@ -4029,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>51</v>
@@ -4104,7 +4104,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>48</v>
@@ -7601,7 +7601,7 @@
       </c>
       <c r="G2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M$3:M$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A2)</f>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="0"/>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="G4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L$3:L$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M$3:M$1048576,'Sprint 1 stats - DO NOT CHANGE'!$A4)</f>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="G10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M1048576,'Sprint 1 stats - DO NOT CHANGE'!$A10)</f>
@@ -7785,8 +7785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="A18:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8319,7 +8319,7 @@
         <v>26</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
@@ -8363,7 +8363,7 @@
         <v>26</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -8407,7 +8407,7 @@
         <v>26</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
@@ -13953,7 +13953,7 @@
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -13966,7 +13966,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>
@@ -19764,7 +19764,7 @@
       </c>
       <c r="D7" s="1">
         <f>COUNTIF('Sprint 1 backlog'!L3:L23,"Done")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -19777,7 +19777,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <f>COUNTIF('Sprint 1 backlog'!M3:M23,"Done")</f>
@@ -20352,6 +20352,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100368EC63562010C468CBEB7AB90BFA937" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbcd4c9f600c040763b05b627a98747d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5517439e-c63d-4269-a460-349c4f0e575b" xmlns:ns3="d12b44e9-a355-4801-8c10-af0fa875eb52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f3ca6a824aa0a87c5592ba6780ee9405" ns2:_="" ns3:_="">
     <xsd:import namespace="5517439e-c63d-4269-a460-349c4f0e575b"/>
@@ -20534,15 +20543,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
   <ds:schemaRefs>
@@ -20555,6 +20555,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{759CF7A7-ED7B-4C51-82F1-9078416C083C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20571,12 +20579,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>